<commit_message>
chore: archive existing progress
</commit_message>
<xml_diff>
--- a/analyze/quickboard.xlsx
+++ b/analyze/quickboard.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ASE2022\UsabilityTest\analyze\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12E94BB2-0D9B-4EEB-826F-49376AE6FED4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45AC013D-8DE9-4A3E-89EF-9D6E030F35C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24675" yWindow="75" windowWidth="21270" windowHeight="13725" firstSheet="10" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Time-LoC-Java" sheetId="4" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -31120,7 +31120,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{D2B81218-A6FD-4FC0-BDAE-C3013F379D6A}">
   <sheetPr codeName="Chart10"/>
   <sheetViews>
-    <sheetView zoomScale="118" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="107" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -31178,7 +31178,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{3BE4B816-75FC-4E63-B769-AD5A49AA2AA8}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="118" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="107" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -31201,7 +31201,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{0FA2D8FC-9C6B-4785-B4A3-E99C2498723D}">
   <sheetPr codeName="Chart8"/>
   <sheetViews>
-    <sheetView zoomScale="318" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="241" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="120" orientation="landscape" r:id="rId1"/>
@@ -31213,7 +31213,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{A84B66DE-2B68-4D2C-B8C7-8ECA7CA7E7CC}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="118" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="107" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -31257,7 +31257,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9298983" cy="6078242"/>
+    <xdr:ext cx="9311355" cy="6079977"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -31422,7 +31422,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9295827" cy="6073083"/>
+    <xdr:ext cx="9299408" cy="6074276"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -31488,7 +31488,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="4082571" cy="2189552"/>
+    <xdr:ext cx="4082707" cy="2189564"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="图表 1">
@@ -31521,7 +31521,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9295827" cy="6073083"/>
+    <xdr:ext cx="9311355" cy="6079977"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -44815,8 +44815,8 @@
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:E300"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -44833,7 +44833,7 @@
         <v>0</v>
       </c>
       <c r="E1" cm="1">
-        <f t="array" ref="E1:E14">FREQUENCY(A1:A100,D1:D13)</f>
+        <f t="array" ref="E1:E14">FREQUENCY(A1:A300,D1:D13)</f>
         <v>1</v>
       </c>
     </row>
@@ -44845,7 +44845,7 @@
         <v>500000</v>
       </c>
       <c r="E2">
-        <v>91</v>
+        <v>271</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -44856,7 +44856,7 @@
         <v>1000000</v>
       </c>
       <c r="E3">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -44867,7 +44867,7 @@
         <v>1500000</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -44878,7 +44878,7 @@
         <v>2000000</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -44933,7 +44933,7 @@
         <v>4500000</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -44966,7 +44966,7 @@
         <v>6000000</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>